<commit_message>
update template barang data
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>kategori_id</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>barang_nama</t>
+  </si>
+  <si>
+    <t>supplier_id</t>
   </si>
   <si>
     <t>harga_beli</t>
@@ -340,21 +343,27 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
         <v>1.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E3" s="2">
         <v>2000.0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>25000.0</v>
       </c>
     </row>
@@ -363,15 +372,18 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="2">
         <v>11500.0</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>12500.0</v>
       </c>
     </row>
@@ -380,15 +392,18 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="2">
         <v>17500.0</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>18500.0</v>
       </c>
     </row>
@@ -397,15 +412,18 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="2">
         <v>89000.0</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>92500.0</v>
       </c>
     </row>
@@ -414,15 +432,18 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="2">
         <v>3750.0</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>4300.0</v>
       </c>
     </row>

</xml_diff>